<commit_message>
09 03 - doxygen
</commit_message>
<xml_diff>
--- a/Documentation/Tabelas-Relatório.xlsx
+++ b/Documentation/Tabelas-Relatório.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Projeto\InteligentDestiller\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAC5AEF-266A-4F65-976E-04657B5A7B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A55BEB-B30C-43A3-A12E-9F5F0AD2505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E0869681-22DC-4313-AFD7-6FC19661AB2B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E0869681-22DC-4313-AFD7-6FC19661AB2B}"/>
   </bookViews>
   <sheets>
     <sheet name="GPIOs" sheetId="2" r:id="rId1"/>
     <sheet name="IOs" sheetId="3" r:id="rId2"/>
-    <sheet name="Esq Eletrico" sheetId="5" r:id="rId3"/>
-    <sheet name="placa ensaio" sheetId="4" r:id="rId4"/>
+    <sheet name="Placa Ensaio" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
   <si>
     <t>GPIO</t>
   </si>
@@ -147,9 +146,6 @@
   </si>
   <si>
     <t>PIN_IND_MAN</t>
-  </si>
-  <si>
-    <t>Componente</t>
   </si>
   <si>
     <t>Descrição</t>
@@ -623,72 +619,6 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3" descr="Table&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5458C639-5C09-9679-46B8-4A39F52F5050}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10201275" y="4038600"/>
-          <a:ext cx="5886450" cy="1438275"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1067,17 +997,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5D67CB-C2A6-4E80-885A-CB555FFEA0C2}">
   <dimension ref="D4:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25:G28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="71.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="71.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <v>0</v>
       </c>
@@ -1119,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <v>1</v>
       </c>
@@ -1133,7 +1063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <v>2</v>
       </c>
@@ -1147,7 +1077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <v>3</v>
       </c>
@@ -1161,7 +1091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <v>4</v>
       </c>
@@ -1173,7 +1103,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <v>5</v>
       </c>
@@ -1187,7 +1117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>6</v>
       </c>
@@ -1201,7 +1131,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <v>7</v>
       </c>
@@ -1215,7 +1145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <v>8</v>
       </c>
@@ -1229,7 +1159,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <v>9</v>
       </c>
@@ -1243,7 +1173,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <v>10</v>
       </c>
@@ -1257,7 +1187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <v>11</v>
       </c>
@@ -1271,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <v>12</v>
       </c>
@@ -1285,7 +1215,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <v>13</v>
       </c>
@@ -1297,7 +1227,7 @@
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <v>14</v>
       </c>
@@ -1311,7 +1241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <v>15</v>
       </c>
@@ -1325,7 +1255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <v>16</v>
       </c>
@@ -1337,7 +1267,7 @@
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <v>17</v>
       </c>
@@ -1349,7 +1279,7 @@
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <v>18</v>
       </c>
@@ -1361,7 +1291,7 @@
       </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <v>19</v>
       </c>
@@ -1373,7 +1303,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <v>21</v>
       </c>
@@ -1385,7 +1315,7 @@
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <v>22</v>
       </c>
@@ -1397,7 +1327,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <v>23</v>
       </c>
@@ -1409,7 +1339,7 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <v>25</v>
       </c>
@@ -1421,7 +1351,7 @@
       </c>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <v>26</v>
       </c>
@@ -1433,7 +1363,7 @@
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <v>27</v>
       </c>
@@ -1445,7 +1375,7 @@
       </c>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <v>32</v>
       </c>
@@ -1457,7 +1387,7 @@
       </c>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <v>33</v>
       </c>
@@ -1469,7 +1399,7 @@
       </c>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <v>34</v>
       </c>
@@ -1481,7 +1411,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <v>35</v>
       </c>
@@ -1493,7 +1423,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <v>36</v>
       </c>
@@ -1505,7 +1435,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <v>39</v>
       </c>
@@ -1531,23 +1461,23 @@
   <dimension ref="B3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H13"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4"/>
-    <col min="2" max="2" width="10.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="4"/>
-    <col min="6" max="6" width="10.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="10.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="10.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1567,27 +1497,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>14</v>
       </c>
@@ -1595,7 +1525,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="6">
         <v>4</v>
@@ -1604,10 +1534,10 @@
         <v>27</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>25</v>
       </c>
@@ -1615,7 +1545,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="6">
         <v>5</v>
@@ -1624,10 +1554,10 @@
         <v>28</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>26</v>
       </c>
@@ -1644,10 +1574,10 @@
         <v>29</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>27</v>
       </c>
@@ -1655,7 +1585,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="6">
         <v>18</v>
@@ -1664,10 +1594,10 @@
         <v>30</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>32</v>
       </c>
@@ -1675,7 +1605,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" s="6">
         <v>19</v>
@@ -1684,10 +1614,10 @@
         <v>31</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F10" s="6">
         <v>21</v>
       </c>
@@ -1695,10 +1625,10 @@
         <v>32</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F11" s="6">
         <v>22</v>
       </c>
@@ -1706,10 +1636,10 @@
         <v>33</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F12" s="6">
         <v>23</v>
       </c>
@@ -1717,10 +1647,10 @@
         <v>34</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F13" s="6">
         <v>33</v>
       </c>
@@ -1728,15 +1658,14 @@
         <v>35</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1746,21 +1675,21 @@
   <dimension ref="C5:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
     <col min="5" max="5" width="22" style="10" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" customWidth="1"/>
-    <col min="16383" max="16384" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
+    <col min="16383" max="16384" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>17</v>
       </c>
@@ -1774,161 +1703,161 @@
         <v>20</v>
       </c>
       <c r="G5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="F6" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="H6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="11"/>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="4">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
         <v>2</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H27" s="10"/>
     </row>
   </sheetData>
@@ -1937,27 +1866,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890A266C-2EFB-4DB9-BBE4-3F0A43108619}">
-  <dimension ref="C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>